<commit_message>
DenseNet in mxnet.gluon for deeplearning
</commit_message>
<xml_diff>
--- a/densenet-gluon/DenseNetParam.xlsx
+++ b/densenet-gluon/DenseNetParam.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="53">
   <si>
     <t>Input_data</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -108,485 +108,591 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>(32, 32)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mx.init.Xavier()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(net.collect_params(), </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11.3"/>
+        <color rgb="FF008080"/>
+        <rFont val="Inconsolata"/>
+        <family val="2"/>
+      </rPr>
+      <t>'adagrad'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.3"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inconsolata"/>
+        <family val="2"/>
+      </rPr>
+      <t>, {</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11.3"/>
+        <color rgb="FF008080"/>
+        <rFont val="Inconsolata"/>
+        <family val="2"/>
+      </rPr>
+      <t>'learning_rate'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.3"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inconsolata"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.3"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Inconsolata"/>
+        <family val="2"/>
+      </rPr>
+      <t>0.01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.3"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inconsolata"/>
+        <family val="2"/>
+      </rPr>
+      <t>})</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(net.collect_params(), </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11.3"/>
+        <color rgb="FF008080"/>
+        <rFont val="Inconsolata"/>
+        <family val="2"/>
+      </rPr>
+      <t>'rmsprop'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.3"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inconsolata"/>
+        <family val="2"/>
+      </rPr>
+      <t>, {</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11.3"/>
+        <color rgb="FF008080"/>
+        <rFont val="Inconsolata"/>
+        <family val="2"/>
+      </rPr>
+      <t>'gamma1'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.3"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inconsolata"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.3"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Inconsolata"/>
+        <family val="2"/>
+      </rPr>
+      <t>0.9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.3"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inconsolata"/>
+        <family val="2"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11.3"/>
+        <color rgb="FF008080"/>
+        <rFont val="Inconsolata"/>
+        <family val="2"/>
+      </rPr>
+      <t>'learning_rate'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.3"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inconsolata"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.3"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Inconsolata"/>
+        <family val="2"/>
+      </rPr>
+      <t>0.01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.3"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inconsolata"/>
+        <family val="2"/>
+      </rPr>
+      <t>})</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(net.collect_params(), </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11.3"/>
+        <color rgb="FF008080"/>
+        <rFont val="Inconsolata"/>
+        <family val="2"/>
+      </rPr>
+      <t>'sgd'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.3"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inconsolata"/>
+        <family val="2"/>
+      </rPr>
+      <t>, {</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11.3"/>
+        <color rgb="FF008080"/>
+        <rFont val="Inconsolata"/>
+        <family val="2"/>
+      </rPr>
+      <t>'learning_rate'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.3"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inconsolata"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.3"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Inconsolata"/>
+        <family val="2"/>
+      </rPr>
+      <t>0.01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.3"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inconsolata"/>
+        <family val="2"/>
+      </rPr>
+      <t>})</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(net.collect_params(), </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11.3"/>
+        <color rgb="FF008080"/>
+        <rFont val="Inconsolata"/>
+        <family val="2"/>
+      </rPr>
+      <t>'adam'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.3"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inconsolata"/>
+        <family val="2"/>
+      </rPr>
+      <t>, {</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11.3"/>
+        <color rgb="FF008080"/>
+        <rFont val="Inconsolata"/>
+        <family val="2"/>
+      </rPr>
+      <t>'learning_rate'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.3"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inconsolata"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.3"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Inconsolata"/>
+        <family val="2"/>
+      </rPr>
+      <t>0.01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.3"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inconsolata"/>
+        <family val="2"/>
+      </rPr>
+      <t>})</t>
+    </r>
+  </si>
+  <si>
+    <t>Optimization</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(net.collect_params(), </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11.3"/>
+        <color rgb="FF008080"/>
+        <rFont val="Inconsolata"/>
+        <family val="2"/>
+      </rPr>
+      <t>'sgd'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.3"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inconsolata"/>
+        <family val="2"/>
+      </rPr>
+      <t>, {</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11.3"/>
+        <color rgb="FF008080"/>
+        <rFont val="Inconsolata"/>
+        <family val="2"/>
+      </rPr>
+      <t>'momentum'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.3"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inconsolata"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.3"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Inconsolata"/>
+        <family val="2"/>
+      </rPr>
+      <t>0.8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.3"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inconsolata"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11.3"/>
+        <color rgb="FF008080"/>
+        <rFont val="Inconsolata"/>
+        <family val="2"/>
+      </rPr>
+      <t>'learning_rate'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.3"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inconsolata"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.3"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Inconsolata"/>
+        <family val="2"/>
+      </rPr>
+      <t>0.01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.3"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inconsolata"/>
+        <family val="2"/>
+      </rPr>
+      <t>})</t>
+    </r>
+  </si>
+  <si>
+    <t>sgd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>adam</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>momentum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>adagrad</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rmsprop</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>adadelta</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(net.collect_params(), </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11.3"/>
+        <color rgb="FF008080"/>
+        <rFont val="Inconsolata"/>
+        <family val="2"/>
+      </rPr>
+      <t>'adadelta'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.3"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inconsolata"/>
+        <family val="2"/>
+      </rPr>
+      <t>, {</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11.3"/>
+        <color rgb="FF008080"/>
+        <rFont val="Inconsolata"/>
+        <family val="2"/>
+      </rPr>
+      <t>'rho'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.3"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inconsolata"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.3"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Inconsolata"/>
+        <family val="2"/>
+      </rPr>
+      <t>0.9999</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.3"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inconsolata"/>
+        <family val="2"/>
+      </rPr>
+      <t>})</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mx.init.Xavier(magnitude=1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(net.collect_params(), </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11.3"/>
+        <color rgb="FF008080"/>
+        <rFont val="Inconsolata"/>
+        <family val="2"/>
+      </rPr>
+      <t>'sgd'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.3"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inconsolata"/>
+        <family val="2"/>
+      </rPr>
+      <t>, {</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11.3"/>
+        <color rgb="FF008080"/>
+        <rFont val="Inconsolata"/>
+        <family val="2"/>
+      </rPr>
+      <t>'learning_rate'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.3"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inconsolata"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.3"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Inconsolata"/>
+        <family val="2"/>
+      </rPr>
+      <t>0.01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.3"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inconsolata"/>
+        <family val="2"/>
+      </rPr>
+      <t>})</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Learning7</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>(32, 32)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>mx.init.Xavier()</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">(net.collect_params(), </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11.3"/>
-        <color rgb="FF008080"/>
-        <rFont val="Inconsolata"/>
-        <family val="2"/>
-      </rPr>
-      <t>'adagrad'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11.3"/>
-        <color rgb="FF000000"/>
-        <rFont val="Inconsolata"/>
-        <family val="2"/>
-      </rPr>
-      <t>, {</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11.3"/>
-        <color rgb="FF008080"/>
-        <rFont val="Inconsolata"/>
-        <family val="2"/>
-      </rPr>
-      <t>'learning_rate'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11.3"/>
-        <color rgb="FF000000"/>
-        <rFont val="Inconsolata"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11.3"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Inconsolata"/>
-        <family val="2"/>
-      </rPr>
-      <t>0.01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11.3"/>
-        <color rgb="FF000000"/>
-        <rFont val="Inconsolata"/>
-        <family val="2"/>
-      </rPr>
-      <t>})</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">(net.collect_params(), </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11.3"/>
-        <color rgb="FF008080"/>
-        <rFont val="Inconsolata"/>
-        <family val="2"/>
-      </rPr>
-      <t>'rmsprop'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11.3"/>
-        <color rgb="FF000000"/>
-        <rFont val="Inconsolata"/>
-        <family val="2"/>
-      </rPr>
-      <t>, {</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11.3"/>
-        <color rgb="FF008080"/>
-        <rFont val="Inconsolata"/>
-        <family val="2"/>
-      </rPr>
-      <t>'gamma1'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11.3"/>
-        <color rgb="FF000000"/>
-        <rFont val="Inconsolata"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11.3"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Inconsolata"/>
-        <family val="2"/>
-      </rPr>
-      <t>0.9</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11.3"/>
-        <color rgb="FF000000"/>
-        <rFont val="Inconsolata"/>
-        <family val="2"/>
-      </rPr>
-      <t>,</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11.3"/>
-        <color rgb="FF008080"/>
-        <rFont val="Inconsolata"/>
-        <family val="2"/>
-      </rPr>
-      <t>'learning_rate'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11.3"/>
-        <color rgb="FF000000"/>
-        <rFont val="Inconsolata"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11.3"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Inconsolata"/>
-        <family val="2"/>
-      </rPr>
-      <t>0.01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11.3"/>
-        <color rgb="FF000000"/>
-        <rFont val="Inconsolata"/>
-        <family val="2"/>
-      </rPr>
-      <t>})</t>
-    </r>
+    <t>Learning8</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">(net.collect_params(), </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11.3"/>
-        <color rgb="FF008080"/>
-        <rFont val="Inconsolata"/>
-        <family val="2"/>
-      </rPr>
-      <t>'sgd'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11.3"/>
-        <color rgb="FF000000"/>
-        <rFont val="Inconsolata"/>
-        <family val="2"/>
-      </rPr>
-      <t>, {</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11.3"/>
-        <color rgb="FF008080"/>
-        <rFont val="Inconsolata"/>
-        <family val="2"/>
-      </rPr>
-      <t>'learning_rate'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11.3"/>
-        <color rgb="FF000000"/>
-        <rFont val="Inconsolata"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11.3"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Inconsolata"/>
-        <family val="2"/>
-      </rPr>
-      <t>0.01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11.3"/>
-        <color rgb="FF000000"/>
-        <rFont val="Inconsolata"/>
-        <family val="2"/>
-      </rPr>
-      <t>})</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">(net.collect_params(), </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11.3"/>
-        <color rgb="FF008080"/>
-        <rFont val="Inconsolata"/>
-        <family val="2"/>
-      </rPr>
-      <t>'adam'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11.3"/>
-        <color rgb="FF000000"/>
-        <rFont val="Inconsolata"/>
-        <family val="2"/>
-      </rPr>
-      <t>, {</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11.3"/>
-        <color rgb="FF008080"/>
-        <rFont val="Inconsolata"/>
-        <family val="2"/>
-      </rPr>
-      <t>'learning_rate'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11.3"/>
-        <color rgb="FF000000"/>
-        <rFont val="Inconsolata"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11.3"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Inconsolata"/>
-        <family val="2"/>
-      </rPr>
-      <t>0.01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11.3"/>
-        <color rgb="FF000000"/>
-        <rFont val="Inconsolata"/>
-        <family val="2"/>
-      </rPr>
-      <t>})</t>
-    </r>
-  </si>
-  <si>
-    <t>Optimization</t>
+    <t>Learning9</t>
+  </si>
+  <si>
+    <t>Learning10</t>
+  </si>
+  <si>
+    <t>Learning11</t>
+  </si>
+  <si>
+    <t>Learning12</t>
+  </si>
+  <si>
+    <t>mx.init.Xavier(magnitude=2)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">(net.collect_params(), </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11.3"/>
-        <color rgb="FF008080"/>
-        <rFont val="Inconsolata"/>
-        <family val="2"/>
-      </rPr>
-      <t>'sgd'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11.3"/>
-        <color rgb="FF000000"/>
-        <rFont val="Inconsolata"/>
-        <family val="2"/>
-      </rPr>
-      <t>, {</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11.3"/>
-        <color rgb="FF008080"/>
-        <rFont val="Inconsolata"/>
-        <family val="2"/>
-      </rPr>
-      <t>'momentum'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11.3"/>
-        <color rgb="FF000000"/>
-        <rFont val="Inconsolata"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11.3"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Inconsolata"/>
-        <family val="2"/>
-      </rPr>
-      <t>0.8</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11.3"/>
-        <color rgb="FF000000"/>
-        <rFont val="Inconsolata"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11.3"/>
-        <color rgb="FF008080"/>
-        <rFont val="Inconsolata"/>
-        <family val="2"/>
-      </rPr>
-      <t>'learning_rate'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11.3"/>
-        <color rgb="FF000000"/>
-        <rFont val="Inconsolata"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11.3"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Inconsolata"/>
-        <family val="2"/>
-      </rPr>
-      <t>0.01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11.3"/>
-        <color rgb="FF000000"/>
-        <rFont val="Inconsolata"/>
-        <family val="2"/>
-      </rPr>
-      <t>})</t>
-    </r>
-  </si>
-  <si>
-    <t>sgd</t>
+    <t>mx.init.Xavier(magnitude=3)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>adam</t>
+    <t>mx.init.Normal(sigma=0.5)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>momentum</t>
+    <t>mx.init.Normal(sigma=1)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>adagrad</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>rmsprop</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>adadelta</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">(net.collect_params(), </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11.3"/>
-        <color rgb="FF008080"/>
-        <rFont val="Inconsolata"/>
-        <family val="2"/>
-      </rPr>
-      <t>'adadelta'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11.3"/>
-        <color rgb="FF000000"/>
-        <rFont val="Inconsolata"/>
-        <family val="2"/>
-      </rPr>
-      <t>, {</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11.3"/>
-        <color rgb="FF008080"/>
-        <rFont val="Inconsolata"/>
-        <family val="2"/>
-      </rPr>
-      <t>'rho'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11.3"/>
-        <color rgb="FF000000"/>
-        <rFont val="Inconsolata"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11.3"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Inconsolata"/>
-        <family val="2"/>
-      </rPr>
-      <t>0.9999</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11.3"/>
-        <color rgb="FF000000"/>
-        <rFont val="Inconsolata"/>
-        <family val="2"/>
-      </rPr>
-      <t>})</t>
-    </r>
+    <t>mx.init.Zero()</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -745,7 +851,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="3.9299758095546984E-2"/>
+          <c:y val="0.15771521639734792"/>
+          <c:w val="0.93632748067211247"/>
+          <c:h val="0.8024687465867858"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -855,7 +971,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-8DAD-4671-ADF7-621C7EEC37DC}"/>
+              <c16:uniqueId val="{00000000-56E2-421A-8955-905673BD35D8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -965,7 +1081,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-8DAD-4671-ADF7-621C7EEC37DC}"/>
+              <c16:uniqueId val="{00000001-56E2-421A-8955-905673BD35D8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1075,7 +1191,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-8DAD-4671-ADF7-621C7EEC37DC}"/>
+              <c16:uniqueId val="{00000002-56E2-421A-8955-905673BD35D8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1185,7 +1301,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-8DAD-4671-ADF7-621C7EEC37DC}"/>
+              <c16:uniqueId val="{00000003-56E2-421A-8955-905673BD35D8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1295,7 +1411,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-8DAD-4671-ADF7-621C7EEC37DC}"/>
+              <c16:uniqueId val="{00000004-56E2-421A-8955-905673BD35D8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1370,34 +1486,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.98</c:v>
+                  <c:v>0.95132211538461497</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.98</c:v>
+                  <c:v>0.98257211538461497</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.98</c:v>
+                  <c:v>0.98257211538461497</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.98</c:v>
+                  <c:v>0.98687900641025605</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.98</c:v>
+                  <c:v>0.98737980769230704</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.98</c:v>
+                  <c:v>0.98407451923076905</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.98</c:v>
+                  <c:v>0.989383012820512</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.98</c:v>
+                  <c:v>0.98768028846153799</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.98</c:v>
+                  <c:v>0.98768028846153799</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.98</c:v>
+                  <c:v>0.99068509615384603</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1405,7 +1521,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-8DAD-4671-ADF7-621C7EEC37DC}"/>
+              <c16:uniqueId val="{00000005-56E2-421A-8955-905673BD35D8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2353,23 +2469,63 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>33132</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>49698</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>4577918</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>976978</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="그림 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="24433697" y="3776872"/>
+          <a:ext cx="4544786" cy="927280"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1088570</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>201704</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1187823</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>67235</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>504265</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>44824</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="차트 5"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvPr id="11" name="차트 10"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -2377,7 +2533,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2692,12 +2848,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:R46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="B16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="topRight" activeCell="D18" sqref="D18"/>
+      <selection pane="topRight" activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -2709,11 +2865,12 @@
     <col min="5" max="5" width="69.125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="55.75" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="70.625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="47.875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="61.75" customWidth="1"/>
+    <col min="9" max="9" width="50.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:18">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
@@ -2734,36 +2891,38 @@
       <c r="H1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>24</v>
-      </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:18">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" s="1"/>
+        <v>24</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="R2" s="1">
+        <v>0.99258814102564097</v>
+      </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:18">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>1</v>
@@ -2786,9 +2945,14 @@
       <c r="H3" s="1">
         <v>64</v>
       </c>
-      <c r="I3" s="1"/>
+      <c r="Q3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="R3" s="2">
+        <v>0.99118589743589702</v>
+      </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:18">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>2</v>
@@ -2803,65 +2967,80 @@
         <v>23</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" s="1"/>
+        <v>25</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="R4" s="1">
+        <v>0.99068509615384603</v>
+      </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:18">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>32</v>
-      </c>
       <c r="F5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="H5" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="I5" s="1"/>
+        <v>38</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="R5" s="1">
+        <v>0.99068509615384603</v>
+      </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:18">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="G6" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="H6" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="H6" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="I6" s="1"/>
+      <c r="Q6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="R6" s="1">
+        <v>0.98958333333333304</v>
+      </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:18">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>3</v>
@@ -2882,9 +3061,14 @@
         <v>0.01</v>
       </c>
       <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
+      <c r="Q7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="R7" s="1">
+        <v>0.98898237179487103</v>
+      </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:18">
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
@@ -2909,9 +3093,8 @@
       <c r="H8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:18">
       <c r="A9" s="4"/>
       <c r="B9" s="1" t="s">
         <v>22</v>
@@ -2932,11 +3115,10 @@
         <v>0.897335737179487</v>
       </c>
       <c r="H9" s="1">
-        <v>0.98</v>
-      </c>
-      <c r="I9" s="1"/>
+        <v>0.95132211538461497</v>
+      </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:18">
       <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
         <v>5</v>
@@ -2957,11 +3139,10 @@
         <v>0.94861778846153799</v>
       </c>
       <c r="H10" s="1">
-        <v>0.98</v>
-      </c>
-      <c r="I10" s="1"/>
+        <v>0.98257211538461497</v>
+      </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:18">
       <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
         <v>6</v>
@@ -2982,11 +3163,10 @@
         <v>0.97215544871794801</v>
       </c>
       <c r="H11" s="1">
-        <v>0.98</v>
-      </c>
-      <c r="I11" s="1"/>
+        <v>0.98257211538461497</v>
+      </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:18">
       <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
         <v>9</v>
@@ -3007,11 +3187,10 @@
         <v>0.97866586538461497</v>
       </c>
       <c r="H12" s="1">
-        <v>0.98</v>
-      </c>
-      <c r="I12" s="1"/>
+        <v>0.98687900641025605</v>
+      </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:18">
       <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
         <v>10</v>
@@ -3032,11 +3211,10 @@
         <v>0.98627804487179405</v>
       </c>
       <c r="H13" s="1">
-        <v>0.98</v>
-      </c>
-      <c r="I13" s="1"/>
+        <v>0.98737980769230704</v>
+      </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:18">
       <c r="A14" s="4"/>
       <c r="B14" s="1" t="s">
         <v>11</v>
@@ -3057,11 +3235,10 @@
         <v>0.98768028846153799</v>
       </c>
       <c r="H14" s="1">
-        <v>0.98</v>
-      </c>
-      <c r="I14" s="1"/>
+        <v>0.98407451923076905</v>
+      </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:18">
       <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
         <v>12</v>
@@ -3082,11 +3259,10 @@
         <v>0.98457532051282004</v>
       </c>
       <c r="H15" s="1">
-        <v>0.98</v>
-      </c>
-      <c r="I15" s="1"/>
+        <v>0.989383012820512</v>
+      </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:18">
       <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
         <v>13</v>
@@ -3107,9 +3283,8 @@
         <v>0.98687900641025605</v>
       </c>
       <c r="H16" s="1">
-        <v>0.98</v>
-      </c>
-      <c r="I16" s="1"/>
+        <v>0.98768028846153799</v>
+      </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="4"/>
@@ -3132,9 +3307,8 @@
         <v>0.98387419871794801</v>
       </c>
       <c r="H17" s="1">
-        <v>0.98</v>
-      </c>
-      <c r="I17" s="1"/>
+        <v>0.98768028846153799</v>
+      </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="5"/>
@@ -3157,12 +3331,358 @@
         <v>0.98898237179487103</v>
       </c>
       <c r="H18" s="1">
-        <v>0.98</v>
-      </c>
-      <c r="I18" s="1"/>
+        <v>0.99068509615384603</v>
+      </c>
     </row>
     <row r="19" spans="1:9" ht="80.25" customHeight="1"/>
+    <row r="29" spans="1:9">
+      <c r="B29" s="1"/>
+      <c r="C29" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="B30" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="B31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" s="1">
+        <v>64</v>
+      </c>
+      <c r="D31" s="1">
+        <v>64</v>
+      </c>
+      <c r="E31" s="1">
+        <v>64</v>
+      </c>
+      <c r="F31" s="1">
+        <v>64</v>
+      </c>
+      <c r="G31" s="1">
+        <v>64</v>
+      </c>
+      <c r="H31" s="1">
+        <v>64</v>
+      </c>
+      <c r="I31" s="1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="B32" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9">
+      <c r="B33" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9">
+      <c r="B34" s="1"/>
+      <c r="C34" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9">
+      <c r="B35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="D35" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="E35" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="F35" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="G35" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="H35" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="I35" s="1">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9">
+      <c r="B36" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9">
+      <c r="B37" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C37" s="1">
+        <v>0.98357371794871795</v>
+      </c>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="5"/>
+    </row>
+    <row r="38" spans="2:9">
+      <c r="B38" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" s="1">
+        <v>0.98968349358974295</v>
+      </c>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
+      <c r="I38" s="5"/>
+    </row>
+    <row r="39" spans="2:9">
+      <c r="B39" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" s="1">
+        <v>0.99198717948717896</v>
+      </c>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
+    </row>
+    <row r="40" spans="2:9">
+      <c r="B40" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40" s="2">
+        <v>0.9921875</v>
+      </c>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
+      <c r="I40" s="5"/>
+    </row>
+    <row r="41" spans="2:9">
+      <c r="B41" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" s="1">
+        <v>0.99298878205128205</v>
+      </c>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
+      <c r="I41" s="5"/>
+    </row>
+    <row r="42" spans="2:9">
+      <c r="B42" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42" s="1">
+        <v>0.99238782051282004</v>
+      </c>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="5"/>
+      <c r="I42" s="5"/>
+    </row>
+    <row r="43" spans="2:9">
+      <c r="B43" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C43" s="1">
+        <v>0.99268830128205099</v>
+      </c>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="5"/>
+      <c r="H43" s="5"/>
+      <c r="I43" s="5"/>
+    </row>
+    <row r="44" spans="2:9">
+      <c r="B44" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C44" s="1">
+        <v>0.99258814102564097</v>
+      </c>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
+      <c r="H44" s="5"/>
+      <c r="I44" s="5"/>
+    </row>
+    <row r="45" spans="2:9">
+      <c r="B45" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C45" s="1">
+        <v>0.99248798076922995</v>
+      </c>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="5"/>
+    </row>
+    <row r="46" spans="2:9">
+      <c r="B46" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C46" s="1">
+        <v>0.99258814102564097</v>
+      </c>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="5"/>
+      <c r="H46" s="5"/>
+      <c r="I46" s="5"/>
+    </row>
   </sheetData>
+  <sortState ref="Q2:R7">
+    <sortCondition descending="1" ref="R7"/>
+  </sortState>
   <mergeCells count="1">
     <mergeCell ref="A8:A17"/>
   </mergeCells>

</xml_diff>